<commit_message>
created classes to represent excel sections
</commit_message>
<xml_diff>
--- a/Solver.xlsx
+++ b/Solver.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Enrollment">'Decision Vars_ Perf. Measures'!$A$2:$C$22</definedName>
     <definedName name="grb_async_callbacks" localSheetId="0" hidden="1">1</definedName>
     <definedName name="grb_bariter" localSheetId="0" hidden="1">1E+100</definedName>
     <definedName name="grb_bartol" localSheetId="0" hidden="1">0.00000001</definedName>
@@ -73,7 +74,7 @@
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_obc" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_obp" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Decision Vars_ Perf. Measures'!$G$11</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Decision Vars_ Perf. Measures'!$G$12</definedName>
     <definedName name="solver_opt_ob" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_psi" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rdp" localSheetId="0" hidden="1">0</definedName>
@@ -104,6 +105,7 @@
     <definedName name="solver_vol" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_vst" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_vst1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="Weights">'Decision Vars_ Perf. Measures'!$M$13:$O$18</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -118,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="87">
   <si>
     <t>Decision Variables</t>
   </si>
@@ -321,9 +323,6 @@
     <t>T TH</t>
   </si>
   <si>
-    <t>MWF</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -374,14 +373,23 @@
   <si>
     <t>morning</t>
   </si>
+  <si>
+    <t>Satisfaction MW</t>
+  </si>
+  <si>
+    <t>Preference for M W</t>
+  </si>
+  <si>
+    <t>M W</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
-    <numFmt numFmtId="168" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -508,9 +516,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -803,8 +811,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:FQ146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1015,22 +1023,22 @@
         <v>3</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>59</v>
       </c>
       <c r="R6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="S6" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="T6" s="12" t="s">
         <v>66</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.5">
@@ -1044,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="H7" s="8">
         <f>SUMPRODUCT($C$3:$C$22,S7:S26)</f>
@@ -1123,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N8" s="9">
         <v>6</v>
@@ -1220,6 +1228,16 @@
       <c r="C10" s="7">
         <v>0</v>
       </c>
+      <c r="F10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="9"/>
       <c r="M10" s="6" t="s">
         <v>61</v>
       </c>
@@ -1259,13 +1277,11 @@
       <c r="C11" s="7">
         <v>0</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="8">
-        <f>SUMPRODUCT(I6:J9,N13:O16)</f>
-        <v>0</v>
-      </c>
+      <c r="M11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="17"/>
+      <c r="O11" s="12"/>
       <c r="Q11" s="6" t="s">
         <v>5</v>
       </c>
@@ -1296,14 +1312,12 @@
       <c r="C12" s="7">
         <v>0</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>64</v>
+      <c r="F12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="8">
+        <f>SUMPRODUCT(I6:J9,N14:O17)</f>
+        <v>0</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>6</v>
@@ -1335,21 +1349,14 @@
       <c r="C13" s="7">
         <v>0</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="6">
-        <f>SUM(C3:C22)</f>
-        <v>0</v>
-      </c>
       <c r="M13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13" s="9">
-        <v>2</v>
-      </c>
-      <c r="O13" s="9">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>7</v>
@@ -1381,11 +1388,18 @@
       <c r="C14" s="7">
         <v>0</v>
       </c>
-      <c r="M14" s="12" t="s">
-        <v>84</v>
+      <c r="F14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="6">
+        <f>SUM(C3:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="N14" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" s="9">
         <v>1</v>
@@ -1420,11 +1434,11 @@
       <c r="C15" s="7">
         <v>0</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>66</v>
+      <c r="M15" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="N15" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O15" s="9">
         <v>1</v>
@@ -1460,13 +1474,13 @@
         <v>0</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N16" s="9">
+        <v>6</v>
+      </c>
+      <c r="O16" s="9">
         <v>1</v>
-      </c>
-      <c r="O16" s="9">
-        <v>2</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>10</v>
@@ -1498,6 +1512,15 @@
       <c r="C17" s="7">
         <v>0</v>
       </c>
+      <c r="M17" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N17" s="9">
+        <v>1</v>
+      </c>
+      <c r="O17" s="9">
+        <v>2</v>
+      </c>
       <c r="Q17" s="6" t="s">
         <v>11</v>
       </c>
@@ -1528,6 +1551,11 @@
       <c r="C18" s="7">
         <v>0</v>
       </c>
+      <c r="M18" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
       <c r="Q18" s="6" t="s">
         <v>12</v>
       </c>
@@ -1781,7 +1809,7 @@
     </row>
     <row r="33" spans="1:173" x14ac:dyDescent="0.5">
       <c r="A33" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13">
@@ -2292,10 +2320,10 @@
         <v>0.91666666666667396</v>
       </c>
       <c r="FP33" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="FQ33" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="FQ33" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:173" x14ac:dyDescent="0.5">
@@ -2483,11 +2511,11 @@
       <c r="FN35" s="17"/>
       <c r="FO35" s="17"/>
       <c r="FP35" s="6">
-        <f>SUM(AY35:FO35)</f>
+        <f t="shared" ref="FP35:FP54" si="4">SUM(AY35:FO35)</f>
         <v>0</v>
       </c>
       <c r="FQ35" s="18">
-        <f>SUM(C35:AX35)</f>
+        <f t="shared" ref="FQ35:FQ54" si="5">SUM(C35:AX35)</f>
         <v>0</v>
       </c>
     </row>
@@ -2668,11 +2696,11 @@
       <c r="FN36" s="17"/>
       <c r="FO36" s="17"/>
       <c r="FP36" s="6">
-        <f>SUM(AY36:FO36)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ36" s="18">
-        <f>SUM(C36:AX36)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2853,11 +2881,11 @@
       <c r="FN37" s="17"/>
       <c r="FO37" s="17"/>
       <c r="FP37" s="6">
-        <f>SUM(AY37:FO37)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ37" s="18">
-        <f>SUM(C37:AX37)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3038,11 +3066,11 @@
       <c r="FN38" s="17"/>
       <c r="FO38" s="17"/>
       <c r="FP38" s="6">
-        <f>SUM(AY38:FO38)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ38" s="18">
-        <f>SUM(C38:AX38)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3223,11 +3251,11 @@
       <c r="FN39" s="17"/>
       <c r="FO39" s="17"/>
       <c r="FP39" s="6">
-        <f>SUM(AY39:FO39)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ39" s="18">
-        <f>SUM(C39:AX39)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3408,11 +3436,11 @@
       <c r="FN40" s="17"/>
       <c r="FO40" s="17"/>
       <c r="FP40" s="6">
-        <f>SUM(AY40:FO40)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ40" s="18">
-        <f>SUM(C40:AX40)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3593,11 +3621,11 @@
       <c r="FN41" s="17"/>
       <c r="FO41" s="17"/>
       <c r="FP41" s="6">
-        <f>SUM(AY41:FO41)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ41" s="18">
-        <f>SUM(C41:AX41)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3778,11 +3806,11 @@
       <c r="FN42" s="17"/>
       <c r="FO42" s="17"/>
       <c r="FP42" s="6">
-        <f>SUM(AY42:FO42)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ42" s="18">
-        <f>SUM(C42:AX42)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -3963,11 +3991,11 @@
       <c r="FN43" s="17"/>
       <c r="FO43" s="17"/>
       <c r="FP43" s="6">
-        <f>SUM(AY43:FO43)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ43" s="18">
-        <f>SUM(C43:AX43)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4148,11 +4176,11 @@
       <c r="FN44" s="17"/>
       <c r="FO44" s="17"/>
       <c r="FP44" s="6">
-        <f>SUM(AY44:FO44)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ44" s="18">
-        <f>SUM(C44:AX44)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4333,11 +4361,11 @@
       <c r="FN45" s="17"/>
       <c r="FO45" s="17"/>
       <c r="FP45" s="6">
-        <f>SUM(AY45:FO45)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ45" s="18">
-        <f>SUM(C45:AX45)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4518,11 +4546,11 @@
       <c r="FN46" s="17"/>
       <c r="FO46" s="17"/>
       <c r="FP46" s="6">
-        <f>SUM(AY46:FO46)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ46" s="18">
-        <f>SUM(C46:AX46)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4703,11 +4731,11 @@
       <c r="FN47" s="17"/>
       <c r="FO47" s="17"/>
       <c r="FP47" s="6">
-        <f>SUM(AY47:FO47)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ47" s="18">
-        <f>SUM(C47:AX47)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4888,11 +4916,11 @@
       <c r="FN48" s="17"/>
       <c r="FO48" s="17"/>
       <c r="FP48" s="6">
-        <f>SUM(AY48:FO48)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ48" s="18">
-        <f>SUM(C48:AX48)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5073,11 +5101,11 @@
       <c r="FN49" s="17"/>
       <c r="FO49" s="17"/>
       <c r="FP49" s="6">
-        <f>SUM(AY49:FO49)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ49" s="18">
-        <f>SUM(C49:AX49)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5258,11 +5286,11 @@
       <c r="FN50" s="17"/>
       <c r="FO50" s="17"/>
       <c r="FP50" s="6">
-        <f>SUM(AY50:FO50)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ50" s="18">
-        <f>SUM(C50:AX50)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5443,11 +5471,11 @@
       <c r="FN51" s="17"/>
       <c r="FO51" s="17"/>
       <c r="FP51" s="6">
-        <f>SUM(AY51:FO51)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ51" s="18">
-        <f>SUM(C51:AX51)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5628,11 +5656,11 @@
       <c r="FN52" s="17"/>
       <c r="FO52" s="17"/>
       <c r="FP52" s="6">
-        <f>SUM(AY52:FO52)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ52" s="18">
-        <f>SUM(C52:AX52)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5813,11 +5841,11 @@
       <c r="FN53" s="17"/>
       <c r="FO53" s="17"/>
       <c r="FP53" s="6">
-        <f>SUM(AY53:FO53)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ53" s="18">
-        <f>SUM(C53:AX53)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5998,11 +6026,11 @@
       <c r="FN54" s="17"/>
       <c r="FO54" s="17"/>
       <c r="FP54" s="6">
-        <f>SUM(AY54:FO54)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="FQ54" s="18">
-        <f>SUM(C54:AX54)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6012,7 +6040,7 @@
     </row>
     <row r="56" spans="1:173" x14ac:dyDescent="0.5">
       <c r="A56" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="13">
@@ -6523,10 +6551,10 @@
         <v>0.91666666666667396</v>
       </c>
       <c r="FP56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="FQ56" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="FQ56" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:173" x14ac:dyDescent="0.5">
@@ -6714,11 +6742,11 @@
       <c r="FN58" s="17"/>
       <c r="FO58" s="17"/>
       <c r="FP58" s="6">
-        <f>SUM(AY58:FO58)</f>
+        <f t="shared" ref="FP58:FP77" si="6">SUM(AY58:FO58)</f>
         <v>0</v>
       </c>
       <c r="FQ58" s="18">
-        <f>SUM(C58:AX58)</f>
+        <f t="shared" ref="FQ58:FQ77" si="7">SUM(C58:AX58)</f>
         <v>0</v>
       </c>
     </row>
@@ -6899,11 +6927,11 @@
       <c r="FN59" s="17"/>
       <c r="FO59" s="17"/>
       <c r="FP59" s="6">
-        <f>SUM(AY59:FO59)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ59" s="18">
-        <f>SUM(C59:AX59)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7084,11 +7112,11 @@
       <c r="FN60" s="17"/>
       <c r="FO60" s="17"/>
       <c r="FP60" s="6">
-        <f>SUM(AY60:FO60)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ60" s="18">
-        <f>SUM(C60:AX60)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7269,11 +7297,11 @@
       <c r="FN61" s="17"/>
       <c r="FO61" s="17"/>
       <c r="FP61" s="6">
-        <f>SUM(AY61:FO61)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ61" s="18">
-        <f>SUM(C61:AX61)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7454,11 +7482,11 @@
       <c r="FN62" s="17"/>
       <c r="FO62" s="17"/>
       <c r="FP62" s="6">
-        <f>SUM(AY62:FO62)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ62" s="18">
-        <f>SUM(C62:AX62)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7639,11 +7667,11 @@
       <c r="FN63" s="17"/>
       <c r="FO63" s="17"/>
       <c r="FP63" s="6">
-        <f>SUM(AY63:FO63)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ63" s="18">
-        <f>SUM(C63:AX63)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7824,11 +7852,11 @@
       <c r="FN64" s="17"/>
       <c r="FO64" s="17"/>
       <c r="FP64" s="6">
-        <f>SUM(AY64:FO64)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ64" s="18">
-        <f>SUM(C64:AX64)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8009,11 +8037,11 @@
       <c r="FN65" s="17"/>
       <c r="FO65" s="17"/>
       <c r="FP65" s="6">
-        <f>SUM(AY65:FO65)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ65" s="18">
-        <f>SUM(C65:AX65)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8194,11 +8222,11 @@
       <c r="FN66" s="17"/>
       <c r="FO66" s="17"/>
       <c r="FP66" s="6">
-        <f>SUM(AY66:FO66)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ66" s="18">
-        <f>SUM(C66:AX66)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8379,11 +8407,11 @@
       <c r="FN67" s="17"/>
       <c r="FO67" s="17"/>
       <c r="FP67" s="6">
-        <f>SUM(AY67:FO67)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ67" s="18">
-        <f>SUM(C67:AX67)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8564,11 +8592,11 @@
       <c r="FN68" s="17"/>
       <c r="FO68" s="17"/>
       <c r="FP68" s="6">
-        <f>SUM(AY68:FO68)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ68" s="18">
-        <f>SUM(C68:AX68)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8749,11 +8777,11 @@
       <c r="FN69" s="17"/>
       <c r="FO69" s="17"/>
       <c r="FP69" s="6">
-        <f>SUM(AY69:FO69)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ69" s="18">
-        <f>SUM(C69:AX69)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8934,11 +8962,11 @@
       <c r="FN70" s="17"/>
       <c r="FO70" s="17"/>
       <c r="FP70" s="6">
-        <f>SUM(AY70:FO70)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ70" s="18">
-        <f>SUM(C70:AX70)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9119,11 +9147,11 @@
       <c r="FN71" s="17"/>
       <c r="FO71" s="17"/>
       <c r="FP71" s="6">
-        <f>SUM(AY71:FO71)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ71" s="18">
-        <f>SUM(C71:AX71)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9304,11 +9332,11 @@
       <c r="FN72" s="17"/>
       <c r="FO72" s="17"/>
       <c r="FP72" s="6">
-        <f>SUM(AY72:FO72)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ72" s="18">
-        <f>SUM(C72:AX72)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9489,11 +9517,11 @@
       <c r="FN73" s="17"/>
       <c r="FO73" s="17"/>
       <c r="FP73" s="6">
-        <f>SUM(AY73:FO73)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ73" s="18">
-        <f>SUM(C73:AX73)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9674,11 +9702,11 @@
       <c r="FN74" s="17"/>
       <c r="FO74" s="17"/>
       <c r="FP74" s="6">
-        <f>SUM(AY74:FO74)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ74" s="18">
-        <f>SUM(C74:AX74)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9859,11 +9887,11 @@
       <c r="FN75" s="17"/>
       <c r="FO75" s="17"/>
       <c r="FP75" s="6">
-        <f>SUM(AY75:FO75)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ75" s="18">
-        <f>SUM(C75:AX75)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10044,11 +10072,11 @@
       <c r="FN76" s="17"/>
       <c r="FO76" s="17"/>
       <c r="FP76" s="6">
-        <f>SUM(AY76:FO76)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ76" s="18">
-        <f>SUM(C76:AX76)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10229,17 +10257,17 @@
       <c r="FN77" s="17"/>
       <c r="FO77" s="17"/>
       <c r="FP77" s="6">
-        <f>SUM(AY77:FO77)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="FQ77" s="18">
-        <f>SUM(C77:AX77)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:173" x14ac:dyDescent="0.5">
       <c r="A79" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="13">
@@ -10750,10 +10778,10 @@
         <v>0.91666666666667396</v>
       </c>
       <c r="FP79" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="FQ79" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="FQ79" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:173" x14ac:dyDescent="0.5">
@@ -10941,11 +10969,11 @@
       <c r="FN81" s="17"/>
       <c r="FO81" s="17"/>
       <c r="FP81" s="6">
-        <f>SUM(AY81:FO81)</f>
+        <f t="shared" ref="FP81:FP100" si="8">SUM(AY81:FO81)</f>
         <v>0</v>
       </c>
       <c r="FQ81" s="18">
-        <f>SUM(C81:AX81)</f>
+        <f t="shared" ref="FQ81:FQ100" si="9">SUM(C81:AX81)</f>
         <v>0</v>
       </c>
     </row>
@@ -11126,11 +11154,11 @@
       <c r="FN82" s="17"/>
       <c r="FO82" s="17"/>
       <c r="FP82" s="6">
-        <f>SUM(AY82:FO82)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ82" s="18">
-        <f>SUM(C82:AX82)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -11311,11 +11339,11 @@
       <c r="FN83" s="17"/>
       <c r="FO83" s="17"/>
       <c r="FP83" s="6">
-        <f>SUM(AY83:FO83)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ83" s="18">
-        <f>SUM(C83:AX83)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -11496,11 +11524,11 @@
       <c r="FN84" s="17"/>
       <c r="FO84" s="17"/>
       <c r="FP84" s="6">
-        <f>SUM(AY84:FO84)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ84" s="18">
-        <f>SUM(C84:AX84)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -11681,11 +11709,11 @@
       <c r="FN85" s="17"/>
       <c r="FO85" s="17"/>
       <c r="FP85" s="6">
-        <f>SUM(AY85:FO85)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ85" s="18">
-        <f>SUM(C85:AX85)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -11866,11 +11894,11 @@
       <c r="FN86" s="17"/>
       <c r="FO86" s="17"/>
       <c r="FP86" s="6">
-        <f>SUM(AY86:FO86)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ86" s="18">
-        <f>SUM(C86:AX86)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12051,11 +12079,11 @@
       <c r="FN87" s="17"/>
       <c r="FO87" s="17"/>
       <c r="FP87" s="6">
-        <f>SUM(AY87:FO87)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ87" s="18">
-        <f>SUM(C87:AX87)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12236,11 +12264,11 @@
       <c r="FN88" s="17"/>
       <c r="FO88" s="17"/>
       <c r="FP88" s="6">
-        <f>SUM(AY88:FO88)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ88" s="18">
-        <f>SUM(C88:AX88)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12421,11 +12449,11 @@
       <c r="FN89" s="17"/>
       <c r="FO89" s="17"/>
       <c r="FP89" s="6">
-        <f>SUM(AY89:FO89)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ89" s="18">
-        <f>SUM(C89:AX89)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12606,11 +12634,11 @@
       <c r="FN90" s="17"/>
       <c r="FO90" s="17"/>
       <c r="FP90" s="6">
-        <f>SUM(AY90:FO90)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ90" s="18">
-        <f>SUM(C90:AX90)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12791,11 +12819,11 @@
       <c r="FN91" s="17"/>
       <c r="FO91" s="17"/>
       <c r="FP91" s="6">
-        <f>SUM(AY91:FO91)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ91" s="18">
-        <f>SUM(C91:AX91)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -12976,11 +13004,11 @@
       <c r="FN92" s="17"/>
       <c r="FO92" s="17"/>
       <c r="FP92" s="6">
-        <f>SUM(AY92:FO92)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ92" s="18">
-        <f>SUM(C92:AX92)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -13161,11 +13189,11 @@
       <c r="FN93" s="17"/>
       <c r="FO93" s="17"/>
       <c r="FP93" s="6">
-        <f>SUM(AY93:FO93)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ93" s="18">
-        <f>SUM(C93:AX93)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -13346,11 +13374,11 @@
       <c r="FN94" s="17"/>
       <c r="FO94" s="17"/>
       <c r="FP94" s="6">
-        <f>SUM(AY94:FO94)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ94" s="18">
-        <f>SUM(C94:AX94)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -13531,11 +13559,11 @@
       <c r="FN95" s="17"/>
       <c r="FO95" s="17"/>
       <c r="FP95" s="6">
-        <f>SUM(AY95:FO95)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ95" s="18">
-        <f>SUM(C95:AX95)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -13716,11 +13744,11 @@
       <c r="FN96" s="17"/>
       <c r="FO96" s="17"/>
       <c r="FP96" s="6">
-        <f>SUM(AY96:FO96)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ96" s="18">
-        <f>SUM(C96:AX96)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -13901,11 +13929,11 @@
       <c r="FN97" s="17"/>
       <c r="FO97" s="17"/>
       <c r="FP97" s="6">
-        <f>SUM(AY97:FO97)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ97" s="18">
-        <f>SUM(C97:AX97)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -14086,11 +14114,11 @@
       <c r="FN98" s="17"/>
       <c r="FO98" s="17"/>
       <c r="FP98" s="6">
-        <f>SUM(AY98:FO98)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ98" s="18">
-        <f>SUM(C98:AX98)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -14271,11 +14299,11 @@
       <c r="FN99" s="17"/>
       <c r="FO99" s="17"/>
       <c r="FP99" s="6">
-        <f>SUM(AY99:FO99)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ99" s="18">
-        <f>SUM(C99:AX99)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -14456,17 +14484,17 @@
       <c r="FN100" s="17"/>
       <c r="FO100" s="17"/>
       <c r="FP100" s="6">
-        <f>SUM(AY100:FO100)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="FQ100" s="18">
-        <f>SUM(C100:AX100)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:173" x14ac:dyDescent="0.5">
       <c r="A102" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B102" s="13"/>
       <c r="C102" s="13">
@@ -14977,10 +15005,10 @@
         <v>0.91666666666667396</v>
       </c>
       <c r="FP102" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="FQ102" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="FQ102" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="103" spans="1:173" x14ac:dyDescent="0.5">
@@ -15168,11 +15196,11 @@
       <c r="FN104" s="17"/>
       <c r="FO104" s="17"/>
       <c r="FP104" s="6">
-        <f>SUM(AY104:FO104)</f>
+        <f t="shared" ref="FP104:FP123" si="10">SUM(AY104:FO104)</f>
         <v>0</v>
       </c>
       <c r="FQ104" s="18">
-        <f>SUM(C104:AX104)</f>
+        <f t="shared" ref="FQ104:FQ123" si="11">SUM(C104:AX104)</f>
         <v>0</v>
       </c>
     </row>
@@ -15353,11 +15381,11 @@
       <c r="FN105" s="17"/>
       <c r="FO105" s="17"/>
       <c r="FP105" s="6">
-        <f>SUM(AY105:FO105)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ105" s="18">
-        <f>SUM(C105:AX105)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -15538,11 +15566,11 @@
       <c r="FN106" s="17"/>
       <c r="FO106" s="17"/>
       <c r="FP106" s="6">
-        <f>SUM(AY106:FO106)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ106" s="18">
-        <f>SUM(C106:AX106)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -15723,11 +15751,11 @@
       <c r="FN107" s="17"/>
       <c r="FO107" s="17"/>
       <c r="FP107" s="6">
-        <f>SUM(AY107:FO107)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ107" s="18">
-        <f>SUM(C107:AX107)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -15908,11 +15936,11 @@
       <c r="FN108" s="17"/>
       <c r="FO108" s="17"/>
       <c r="FP108" s="6">
-        <f>SUM(AY108:FO108)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ108" s="18">
-        <f>SUM(C108:AX108)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -16093,11 +16121,11 @@
       <c r="FN109" s="17"/>
       <c r="FO109" s="17"/>
       <c r="FP109" s="6">
-        <f>SUM(AY109:FO109)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ109" s="18">
-        <f>SUM(C109:AX109)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -16278,11 +16306,11 @@
       <c r="FN110" s="17"/>
       <c r="FO110" s="17"/>
       <c r="FP110" s="6">
-        <f>SUM(AY110:FO110)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ110" s="18">
-        <f>SUM(C110:AX110)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -16463,11 +16491,11 @@
       <c r="FN111" s="17"/>
       <c r="FO111" s="17"/>
       <c r="FP111" s="6">
-        <f>SUM(AY111:FO111)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ111" s="18">
-        <f>SUM(C111:AX111)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -16648,11 +16676,11 @@
       <c r="FN112" s="17"/>
       <c r="FO112" s="17"/>
       <c r="FP112" s="6">
-        <f>SUM(AY112:FO112)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ112" s="18">
-        <f>SUM(C112:AX112)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -16833,11 +16861,11 @@
       <c r="FN113" s="17"/>
       <c r="FO113" s="17"/>
       <c r="FP113" s="6">
-        <f>SUM(AY113:FO113)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ113" s="18">
-        <f>SUM(C113:AX113)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -17018,11 +17046,11 @@
       <c r="FN114" s="17"/>
       <c r="FO114" s="17"/>
       <c r="FP114" s="6">
-        <f>SUM(AY114:FO114)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ114" s="18">
-        <f>SUM(C114:AX114)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -17203,11 +17231,11 @@
       <c r="FN115" s="17"/>
       <c r="FO115" s="17"/>
       <c r="FP115" s="6">
-        <f>SUM(AY115:FO115)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ115" s="18">
-        <f>SUM(C115:AX115)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -17388,11 +17416,11 @@
       <c r="FN116" s="17"/>
       <c r="FO116" s="17"/>
       <c r="FP116" s="6">
-        <f>SUM(AY116:FO116)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ116" s="18">
-        <f>SUM(C116:AX116)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -17573,11 +17601,11 @@
       <c r="FN117" s="17"/>
       <c r="FO117" s="17"/>
       <c r="FP117" s="6">
-        <f>SUM(AY117:FO117)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ117" s="18">
-        <f>SUM(C117:AX117)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -17758,11 +17786,11 @@
       <c r="FN118" s="17"/>
       <c r="FO118" s="17"/>
       <c r="FP118" s="6">
-        <f>SUM(AY118:FO118)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ118" s="18">
-        <f>SUM(C118:AX118)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -17943,11 +17971,11 @@
       <c r="FN119" s="17"/>
       <c r="FO119" s="17"/>
       <c r="FP119" s="6">
-        <f>SUM(AY119:FO119)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ119" s="18">
-        <f>SUM(C119:AX119)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -18128,11 +18156,11 @@
       <c r="FN120" s="17"/>
       <c r="FO120" s="17"/>
       <c r="FP120" s="6">
-        <f>SUM(AY120:FO120)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ120" s="18">
-        <f>SUM(C120:AX120)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -18313,11 +18341,11 @@
       <c r="FN121" s="17"/>
       <c r="FO121" s="17"/>
       <c r="FP121" s="6">
-        <f>SUM(AY121:FO121)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ121" s="18">
-        <f>SUM(C121:AX121)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -18498,11 +18526,11 @@
       <c r="FN122" s="17"/>
       <c r="FO122" s="17"/>
       <c r="FP122" s="6">
-        <f>SUM(AY122:FO122)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ122" s="18">
-        <f>SUM(C122:AX122)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -18683,17 +18711,17 @@
       <c r="FN123" s="17"/>
       <c r="FO123" s="17"/>
       <c r="FP123" s="6">
-        <f>SUM(AY123:FO123)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="FQ123" s="18">
-        <f>SUM(C123:AX123)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:173" x14ac:dyDescent="0.5">
       <c r="A125" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B125" s="13"/>
       <c r="C125" s="13">
@@ -19204,10 +19232,10 @@
         <v>0.91666666666667396</v>
       </c>
       <c r="FP125" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="FQ125" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="FQ125" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="126" spans="1:173" x14ac:dyDescent="0.5">
@@ -19395,11 +19423,11 @@
       <c r="FN127" s="17"/>
       <c r="FO127" s="17"/>
       <c r="FP127" s="6">
-        <f>SUM(AY127:FO127)</f>
+        <f t="shared" ref="FP127:FP146" si="12">SUM(AY127:FO127)</f>
         <v>0</v>
       </c>
       <c r="FQ127" s="18">
-        <f>SUM(C127:AX127)</f>
+        <f t="shared" ref="FQ127:FQ146" si="13">SUM(C127:AX127)</f>
         <v>0</v>
       </c>
     </row>
@@ -19580,11 +19608,11 @@
       <c r="FN128" s="17"/>
       <c r="FO128" s="17"/>
       <c r="FP128" s="6">
-        <f>SUM(AY128:FO128)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ128" s="18">
-        <f>SUM(C128:AX128)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -19765,11 +19793,11 @@
       <c r="FN129" s="17"/>
       <c r="FO129" s="17"/>
       <c r="FP129" s="6">
-        <f>SUM(AY129:FO129)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ129" s="18">
-        <f>SUM(C129:AX129)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -19950,11 +19978,11 @@
       <c r="FN130" s="17"/>
       <c r="FO130" s="17"/>
       <c r="FP130" s="6">
-        <f>SUM(AY130:FO130)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ130" s="18">
-        <f>SUM(C130:AX130)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -20135,11 +20163,11 @@
       <c r="FN131" s="17"/>
       <c r="FO131" s="17"/>
       <c r="FP131" s="6">
-        <f>SUM(AY131:FO131)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ131" s="18">
-        <f>SUM(C131:AX131)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -20320,11 +20348,11 @@
       <c r="FN132" s="17"/>
       <c r="FO132" s="17"/>
       <c r="FP132" s="6">
-        <f>SUM(AY132:FO132)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ132" s="18">
-        <f>SUM(C132:AX132)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -20505,11 +20533,11 @@
       <c r="FN133" s="17"/>
       <c r="FO133" s="17"/>
       <c r="FP133" s="6">
-        <f>SUM(AY133:FO133)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ133" s="18">
-        <f>SUM(C133:AX133)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -20690,11 +20718,11 @@
       <c r="FN134" s="17"/>
       <c r="FO134" s="17"/>
       <c r="FP134" s="6">
-        <f>SUM(AY134:FO134)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ134" s="18">
-        <f>SUM(C134:AX134)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -20875,11 +20903,11 @@
       <c r="FN135" s="17"/>
       <c r="FO135" s="17"/>
       <c r="FP135" s="6">
-        <f>SUM(AY135:FO135)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ135" s="18">
-        <f>SUM(C135:AX135)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -21060,11 +21088,11 @@
       <c r="FN136" s="17"/>
       <c r="FO136" s="17"/>
       <c r="FP136" s="6">
-        <f>SUM(AY136:FO136)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ136" s="18">
-        <f>SUM(C136:AX136)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -21245,11 +21273,11 @@
       <c r="FN137" s="17"/>
       <c r="FO137" s="17"/>
       <c r="FP137" s="6">
-        <f>SUM(AY137:FO137)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ137" s="18">
-        <f>SUM(C137:AX137)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -21430,11 +21458,11 @@
       <c r="FN138" s="17"/>
       <c r="FO138" s="17"/>
       <c r="FP138" s="6">
-        <f>SUM(AY138:FO138)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ138" s="18">
-        <f>SUM(C138:AX138)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -21615,11 +21643,11 @@
       <c r="FN139" s="17"/>
       <c r="FO139" s="17"/>
       <c r="FP139" s="6">
-        <f>SUM(AY139:FO139)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ139" s="18">
-        <f>SUM(C139:AX139)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -21800,11 +21828,11 @@
       <c r="FN140" s="17"/>
       <c r="FO140" s="17"/>
       <c r="FP140" s="6">
-        <f>SUM(AY140:FO140)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ140" s="18">
-        <f>SUM(C140:AX140)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -21985,11 +22013,11 @@
       <c r="FN141" s="17"/>
       <c r="FO141" s="17"/>
       <c r="FP141" s="6">
-        <f>SUM(AY141:FO141)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ141" s="18">
-        <f>SUM(C141:AX141)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -22170,11 +22198,11 @@
       <c r="FN142" s="17"/>
       <c r="FO142" s="17"/>
       <c r="FP142" s="6">
-        <f>SUM(AY142:FO142)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ142" s="18">
-        <f>SUM(C142:AX142)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -22355,11 +22383,11 @@
       <c r="FN143" s="17"/>
       <c r="FO143" s="17"/>
       <c r="FP143" s="6">
-        <f>SUM(AY143:FO143)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ143" s="18">
-        <f>SUM(C143:AX143)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -22540,11 +22568,11 @@
       <c r="FN144" s="17"/>
       <c r="FO144" s="17"/>
       <c r="FP144" s="6">
-        <f>SUM(AY144:FO144)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ144" s="18">
-        <f>SUM(C144:AX144)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -22725,11 +22753,11 @@
       <c r="FN145" s="17"/>
       <c r="FO145" s="17"/>
       <c r="FP145" s="6">
-        <f>SUM(AY145:FO145)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ145" s="18">
-        <f>SUM(C145:AX145)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -22910,11 +22938,11 @@
       <c r="FN146" s="17"/>
       <c r="FO146" s="17"/>
       <c r="FP146" s="6">
-        <f>SUM(AY146:FO146)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="FQ146" s="18">
-        <f>SUM(C146:AX146)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -22943,19 +22971,19 @@
         <v>58</v>
       </c>
       <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>71</v>
-      </c>
-      <c r="S1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.5">

</xml_diff>